<commit_message>
pequeños cambios en los nombres de los casos de prueba
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
+++ b/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFBCEC0-34C3-419E-80F0-04A44A67FDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0958868-F21E-4202-9985-D0F25BF6EB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +556,7 @@
     <col min="12" max="12" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
se agrega caso de prueba CP_GESCLSERDOM_004 gestion clientes servicios domiciliarios
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
+++ b/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99066D8C-76D6-4D66-8D51-51842A34AFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79105AA-0E5E-45C3-9885-5DE610776D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>ID Caso</t>
   </si>
@@ -140,6 +140,28 @@
   </si>
   <si>
     <t>se visualizó la información del cliente correctamente</t>
+  </si>
+  <si>
+    <t>CP_GESCLSERDOM_004</t>
+  </si>
+  <si>
+    <t>Reconfiguración 
+del cliente</t>
+  </si>
+  <si>
+    <t>Cliente seleccionado y visible en la tabla</t>
+  </si>
+  <si>
+    <t>1. Clic en Opciones.
+2. Seleccionar Reconfiguración.
+3. Clic en Reconfigurar.
+4. Confirmar en el modal con Sí.</t>
+  </si>
+  <si>
+    <t>Se inicia el proceso de reconfiguración y se muestran barras de progreso.</t>
+  </si>
+  <si>
+    <t>Se visualiza correctamente el proceso de reconfiguracion</t>
   </si>
 </sst>
 </file>
@@ -268,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -298,8 +320,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,7 +609,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,18 +782,42 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="A5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>

</xml_diff>

<commit_message>
se agregan casos de prueba CP_GESCLSERDOM_005 al CP_GESCLSERDOM_008
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
+++ b/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatización v2\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79105AA-0E5E-45C3-9885-5DE610776D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="GestionClientesServiciosDomi" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>ID Caso</t>
   </si>
@@ -163,12 +162,18 @@
   <si>
     <t>Se visualiza correctamente el proceso de reconfiguracion</t>
   </si>
+  <si>
+    <t>CP_GESCLSERDOM_005</t>
+  </si>
+  <si>
+    <t>Ver dispositivos del cliente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -322,9 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,14 +607,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -628,7 +630,7 @@
     <col min="12" max="12" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +668,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="147" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -705,7 +707,7 @@
       </c>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="1:13" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="90.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -743,7 +745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="97.5" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -781,8 +783,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:13" ht="66.75" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -819,9 +821,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+    <row r="6" spans="1:13" ht="143.25" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -833,7 +839,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="180" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="5"/>

</xml_diff>

<commit_message>
se agregan mas casos de prueba en el documento
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
+++ b/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatización v2\Automatizacion\docs\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB130618-CCFB-4A1B-966D-1EEA08D98358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GestionClientesServiciosDomi" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>ID Caso</t>
   </si>
@@ -168,12 +169,46 @@
   <si>
     <t>Ver dispositivos del cliente</t>
   </si>
+  <si>
+    <t>Cliente en estado ACTIVO seleccionado</t>
+  </si>
+  <si>
+    <t>1. Clic en Opciones.
+2. Seleccionar Ver dispositivos.</t>
+  </si>
+  <si>
+    <t>El sistema abre un modal que lista los dispositivos asociados al cliente.</t>
+  </si>
+  <si>
+    <t>el modal se visualiza correctamente</t>
+  </si>
+  <si>
+    <t>CP_GESCLSERDOM_006</t>
+  </si>
+  <si>
+    <t>Ver y enviar documentos (Acta de instalación y Contrato)</t>
+  </si>
+  <si>
+    <t>Cliente con 
+documentos asociados</t>
+  </si>
+  <si>
+    <t>1. Clic en Opciones.
+2. Seleccionar Ver documentos.
+3. Para cada documento:
+ a. Clic Ver documento.
+ b. Clic Enviar al correo.
+ c. Clic Descargar.</t>
+  </si>
+  <si>
+    <t>El sistema abre un modal para visualizar los documentos del cliente(Acta de instalación y Contrato)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -310,12 +345,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -607,14 +638,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -630,7 +661,7 @@
     <col min="12" max="12" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,56 +699,56 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="147" customHeight="1">
+    <row r="2" spans="1:13" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="11"/>
+      <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="90.75" customHeight="1">
+    <row r="3" spans="1:13" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -726,7 +757,7 @@
       <c r="F3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -735,27 +766,27 @@
       <c r="I3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="97.5" customHeight="1">
+    <row r="4" spans="1:13" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -764,7 +795,7 @@
       <c r="F4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -773,17 +804,17 @@
       <c r="I4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="66.75" customHeight="1">
+    <row r="5" spans="1:13" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -811,47 +842,91 @@
       <c r="I5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="143.25" customHeight="1">
+    <row r="6" spans="1:13" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="180" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+    <row r="7" spans="1:13" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
agregando casos de prueba en el documento y ajustando la emnumeracion de los casos de prueba en algunas vistas.
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
+++ b/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB130618-CCFB-4A1B-966D-1EEA08D98358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DDDAC5-B121-4580-AF32-86DA2AF7A25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
   <si>
     <t>ID Caso</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Se inicia el proceso de reconfiguración y se muestran barras de progreso.</t>
   </si>
   <si>
-    <t>Se visualiza correctamente el proceso de reconfiguracion</t>
-  </si>
-  <si>
     <t>CP_GESCLSERDOM_005</t>
   </si>
   <si>
@@ -173,14 +170,7 @@
     <t>Cliente en estado ACTIVO seleccionado</t>
   </si>
   <si>
-    <t>1. Clic en Opciones.
-2. Seleccionar Ver dispositivos.</t>
-  </si>
-  <si>
     <t>El sistema abre un modal que lista los dispositivos asociados al cliente.</t>
-  </si>
-  <si>
-    <t>el modal se visualiza correctamente</t>
   </si>
   <si>
     <t>CP_GESCLSERDOM_006</t>
@@ -202,6 +192,108 @@
   </si>
   <si>
     <t>El sistema abre un modal para visualizar los documentos del cliente(Acta de instalación y Contrato)</t>
+  </si>
+  <si>
+    <t>CP_GESCLSERDOM_007</t>
+  </si>
+  <si>
+    <t>Ver detalle del proceso</t>
+  </si>
+  <si>
+    <t>Cliente seleccionado</t>
+  </si>
+  <si>
+    <t>1. Clic en Opciones.
+2. Seleccionar Detalle del proceso.</t>
+  </si>
+  <si>
+    <t>Se despliega un modal con el historial y detalle de procesos del cliente.</t>
+  </si>
+  <si>
+    <t>El proceso de reconfiguración inició y las barras de progreso se mostraron correctamente.</t>
+  </si>
+  <si>
+    <t>El modal se abrió y mostró la lista de dispositivos asociados.</t>
+  </si>
+  <si>
+    <t>Acta y Contrato se visualizaron, enviaron y descargaron según lo esperado.</t>
+  </si>
+  <si>
+    <t>El modal se abrió y mostró el historial y detalle de procesos correctamente.</t>
+  </si>
+  <si>
+    <t>CP_GESCLSERDOM_008</t>
+  </si>
+  <si>
+    <t>Suspensión del cliente</t>
+  </si>
+  <si>
+    <t>1. Clic en Opciones.
+2. Seleccionar opción "Suspensión"</t>
+  </si>
+  <si>
+    <t>Cliente en estado ACTIVO y con plan vigente.</t>
+  </si>
+  <si>
+    <t>1. Seleccionar cliente.
+2. Clic en Opciones.
+3. Seleccionar Suspensión de servicio.
+4. Confirmar en el modal con botón Sí.</t>
+  </si>
+  <si>
+    <t>El sistema inicia la suspensión, muestra barra de progreso y cambia el estado del cliente a SUSPENDIDO.</t>
+  </si>
+  <si>
+    <t>Suspensión ejecutada y estado del cliente actualizado a SUSPENDIDO.</t>
+  </si>
+  <si>
+    <t>CP_GESCLSERDOM_009</t>
+  </si>
+  <si>
+    <t>Renexion de servicio suspendido</t>
+  </si>
+  <si>
+    <t>Cliente previamente suspendido (Estado = SUSPENDIDO).</t>
+  </si>
+  <si>
+    <t>1. Seleccionar cliente.
+2. Clic en Opciones.
+3. Seleccionar Reconexión de servicio.
+4. Confirmar en el modal con botón Sí.</t>
+  </si>
+  <si>
+    <t>ID de cliente suspendido</t>
+  </si>
+  <si>
+    <t>El sistema reconecta el servicio, muestra barra de progreso y cambia el estado del cliente a ACTIVO.</t>
+  </si>
+  <si>
+    <t>Servicio re-conectado y estado del cliente actualizado a ACTIVO.</t>
+  </si>
+  <si>
+    <t>Cambio de plan de servicio</t>
+  </si>
+  <si>
+    <t>Cliente en estado ACTIVO y con al menos un plan disponible para cambio.</t>
+  </si>
+  <si>
+    <t>1. Seleccionar cliente.
+2. Clic en Opciones.
+3. Seleccionar Cambio de plan.
+4. En el modal, escoger nuevo plan de la lista.
+5. Clic en Guardar/Confirmar cambio.</t>
+  </si>
+  <si>
+    <t>ID de cliente y nombre del nuevo plan</t>
+  </si>
+  <si>
+    <t>El sistema actualiza el plan contratado y muestra confirmación de cambio exitoso.</t>
+  </si>
+  <si>
+    <t>Cambio de plan ejecutado correctamente y plan actualizado.</t>
+  </si>
+  <si>
+    <t>CP_GESCLSERDOM_010</t>
   </si>
 </sst>
 </file>
@@ -639,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -719,7 +811,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>23</v>
@@ -738,7 +830,7 @@
       </c>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -758,7 +850,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>27</v>
@@ -776,7 +868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -840,7 +932,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>20</v>
@@ -852,12 +944,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -866,19 +958,19 @@
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="I6" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>20</v>
@@ -890,12 +982,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -904,19 +996,19 @@
         <v>17</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>20</v>
@@ -925,6 +1017,196 @@
         <v>13</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se realizan nuevos ajustes en diagramas, excel y codigo
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
+++ b/docs/test-cases/gestionClientesServiciosDomiciliarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatización v2\Automatizacion\docs\test-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev Celsia\Automatizacion\docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9172E7-640B-49D0-BD54-078B87F7B6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GestionClientesServiciosDomi" sheetId="1" r:id="rId1"/>
@@ -210,9 +211,6 @@
     <t>CP_GESCLSERDOM_009</t>
   </si>
   <si>
-    <t>Renexion de servicio suspendido</t>
-  </si>
-  <si>
     <t>Cliente previamente suspendido (Estado = SUSPENDIDO).</t>
   </si>
   <si>
@@ -261,13 +259,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1. seleccionar cliente
-2. Botón Opciones
-3. Seleccionar opción "Ver dispositivos"
-4.Cerrar el modal "Ver dispositivos"
-</t>
-  </si>
-  <si>
     <t>1. seleccionar cliente
 2. Botón Opciones.
 3. Seleccionar opción "Ver documentos"
@@ -281,31 +272,6 @@
 3.Seleccionar opción "Detalle del proceso"
 4.Cerrar modal "Detalle del proceso"
 5.deseleccionar cliente</t>
-  </si>
-  <si>
-    <t>1. Seleccionar cliente.
-2. Clic en Opciones.
-3. Seleccionar Reconexión de servicio.
-4. Seleccionar motivo "SUSPENSION POR NO PAGO"
-5.Diligenciar comentario.
-6.Confirmar suspensión
-7.Confirmar con “Sí”
-8.Validar modal de detalle del proceso
-9.Cerrar modal de detalle
-10.deseleccionar cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar cliente.
-2. Clic en Opciones.
-3. Seleccionar opción 'Reconexión'
-4. Diligenciar comentario
-5.Confirmar reconexión
-6.Confirmar con “Sí”
-7.Esperar barra de progreso
-8.Esperar modal de detalle del proceso
-9.Verificar que exista texto de orden de reconexión
-10.Cerrar modal de detalle
-11.deseleccionar cliente </t>
   </si>
   <si>
     <t>1. Seleccionar cliente.
@@ -326,7 +292,48 @@
     <t>Cambio de plan del cliente (dando clic en CANCELAR)</t>
   </si>
   <si>
+    <t>el modal de cambio de plan se cierra exitosamente</t>
+  </si>
+  <si>
+    <t>El sistema no debe actualizar el plan contratado y cierra el modal.</t>
+  </si>
+  <si>
+    <t>ID de un cliente suspendido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. seleccionar cliente
+2. Botón Opciones
+3. Seleccionar opción "Ver dispositivos"
+4.Cerrar el modal "Ver dispositivos"
+5.deseleccionar cliente
+</t>
+  </si>
+  <si>
+    <t>Reconexion de servicio suspendido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar cliente.
+2. Clic en Opciones.
+3. Seleccionar opción 'Reconexión'
+4. Diligenciar comentario
+5.Confirmar reconexión
+6.Confirmar con “Sí”
+7.Cerrar modal de detalle
+8.deseleccionar cliente </t>
+  </si>
+  <si>
     <t>1. Seleccionar cliente.
+2. Clic en Opciones.
+3. Seleccionar opción "Suspensión".
+4. Seleccionar motivo "SUSPENSION POR NO PAGO"
+5.Diligenciar comentario.
+6.Confirmar suspensión
+7.Confirmar con “Sí”
+8.Cerrar modal de detalle
+9.deseleccionar cliente</t>
+  </si>
+  <si>
+    <t>1. Seleccionar cliente por ID_DEAL.
 2. Clic en Opciones.
 3. Seleccionar opción "Cambio de plan"
 4. Clic en botón "Nuevo plan comercial".
@@ -335,21 +342,12 @@
 7.Diligenciar número PQ y comentario
 8.CANCELAR en lugar de Confirmar</t>
   </si>
-  <si>
-    <t>el modal de cambio de plan se cierra exitosamente</t>
-  </si>
-  <si>
-    <t>El sistema no debe actualizar el plan contratado y cierra el modal.</t>
-  </si>
-  <si>
-    <t>ID de un cliente suspendido</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -499,6 +497,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,14 +783,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -802,7 +806,7 @@
     <col min="12" max="12" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -840,7 +844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="98.25" customHeight="1">
+    <row r="2" spans="1:13" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -879,7 +883,7 @@
       </c>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="96" customHeight="1">
+    <row r="3" spans="1:13" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -896,7 +900,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>30</v>
@@ -917,7 +921,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="117.75" customHeight="1">
+    <row r="4" spans="1:13" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -934,7 +938,7 @@
         <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>30</v>
@@ -955,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="66.75" customHeight="1">
+    <row r="5" spans="1:13" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -972,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>30</v>
@@ -993,7 +997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="56.25" customHeight="1">
+    <row r="6" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -1010,7 +1014,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>30</v>
@@ -1031,7 +1035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="94.5" customHeight="1">
+    <row r="7" spans="1:13" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>44</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>14</v>
@@ -1069,7 +1073,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="88.5" customHeight="1">
+    <row r="8" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>30</v>
@@ -1107,7 +1111,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="96" customHeight="1">
+    <row r="9" spans="1:13" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1124,7 +1128,7 @@
         <v>56</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>30</v>
@@ -1145,33 +1149,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="100.5" customHeight="1">
+    <row r="10" spans="1:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>20</v>
@@ -1183,12 +1187,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="193.5" customHeight="1">
+    <row r="11" spans="1:13" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
@@ -1197,19 +1201,19 @@
         <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>20</v>
@@ -1221,12 +1225,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="193.5" customHeight="1">
+    <row r="12" spans="1:13" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>12</v>
@@ -1235,19 +1239,19 @@
         <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>20</v>

</xml_diff>